<commit_message>
update overview file and js file
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Behaviour
 The program should:</t>
@@ -37,13 +37,94 @@
   </si>
   <si>
     <t>Allow user to enter length values of the three sides of the triangle</t>
+  </si>
+  <si>
+    <t>After user submits values, the application should tell user what type of triangle the values will produce, whether an isosceles, equilateral, scalene or NO triangle at all.</t>
+  </si>
+  <si>
+    <t>1. The project uses one or more javascript functions.</t>
+  </si>
+  <si>
+    <t>TECHNICAL REQUIREMENTS:</t>
+  </si>
+  <si>
+    <t>2. Appropriate control flows and logical operators are used in the project.</t>
+  </si>
+  <si>
+    <t>3. The project makes use of one or more arrays in javascript.</t>
+  </si>
+  <si>
+    <t>4. The project uses a  HTML input to collect user data.</t>
+  </si>
+  <si>
+    <t>5. The project uses a custom CSS stylesheet that incorporates cascading, box model and floats.</t>
+  </si>
+  <si>
+    <t>6. The project works as expected, achieving the functionality required.</t>
+  </si>
+  <si>
+    <t>7. The project demonstrates an understanding of the week's concepts. If requested, you should be able to explain your code to your instructor.</t>
+  </si>
+  <si>
+    <t>USER REQUIREMENTS:</t>
+  </si>
+  <si>
+    <t>triangle length from user</t>
+  </si>
+  <si>
+    <t>type of triangle; either isosceles, equilateral, scalene or NO triangle at all.</t>
+  </si>
+  <si>
+    <t>prompt user for lengths</t>
+  </si>
+  <si>
+    <t>Based on the functionality of the application, key points to note are:</t>
+  </si>
+  <si>
+    <t>2. For an isosceles triangle, two sides are exactly equal.</t>
+  </si>
+  <si>
+    <t>3. For a scalene triangle, none of the sides is equal. However, the sum of any two sides of the triangle must be greater than the third side.</t>
+  </si>
+  <si>
+    <t>4. Most importantly, if the sum of any two sides of the triangle is equal to or less than the third remaining side, then a triangle CANNOT be formed using those values. (For example, the values 9,4 &amp; 3 cannot form a triangle.)</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>isosceles</t>
+  </si>
+  <si>
+    <t>equilateral</t>
+  </si>
+  <si>
+    <t>userInput1===userInput2 &amp;&amp; userInput2===userInput3 &amp;&amp; userInput1===userInput3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scalene </t>
+  </si>
+  <si>
+    <t>userInput1 === userInput2 &amp;&amp; userInput3 !== userInput1 &amp;&amp; userInput3!==userInput2</t>
+  </si>
+  <si>
+    <t>userInput2 === userInput3 &amp;&amp; userInput1 !== userInput2 &amp;&amp; userInput1!==userInput3</t>
+  </si>
+  <si>
+    <t>userInput1 === userInput3 &amp;&amp; userInput2 !== userInput1 &amp;&amp; userInput2!==userInput3</t>
+  </si>
+  <si>
+    <t>(userInput1 === userInput2 !== userInput3)||(userInput3===userInput1 !==userInput2)|| (userInput3===userInput2 !==userInput1)</t>
+  </si>
+  <si>
+    <t>or (This takes care of the side that should not be equal to others.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +133,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF2D3B45"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FF2D3B45"/>
       <name val="Helvetica"/>
@@ -78,12 +174,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -366,37 +472,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="9" max="9" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="I2" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the overview file
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Behaviour
 The program should:</t>
@@ -114,10 +115,37 @@
     <t>userInput1 === userInput3 &amp;&amp; userInput2 !== userInput1 &amp;&amp; userInput2!==userInput3</t>
   </si>
   <si>
-    <t>(userInput1 === userInput2 !== userInput3)||(userInput3===userInput1 !==userInput2)|| (userInput3===userInput2 !==userInput1)</t>
-  </si>
-  <si>
-    <t>or (This takes care of the side that should not be equal to others.</t>
+    <t>For a scalene triangle, none of the sides is equal. However, the sum of any two sides of the triangle must be greater than the third side.</t>
+  </si>
+  <si>
+    <t>userInput1!==userInput2 &amp;&amp; userInput2!==userInput3 &amp;&amp; userInput1!==userInput3</t>
+  </si>
+  <si>
+    <t>userInput1+userInput2 &gt;userInput3 || userInput1+userInput3 &gt;userInput2 || userInput3+userInput2 &gt;userInput1</t>
+  </si>
+  <si>
+    <t>// For a scalene triangle, none of the sides is equal. However, the sum of any two sides of the triangle must be greater than the third side.</t>
+  </si>
+  <si>
+    <t>var userInput1= parseInt(prompt("Please enter the 1st length of your triangle."));</t>
+  </si>
+  <si>
+    <t>var userInput2= parseInt(prompt("Please enter the 2nd length of your triangle."));</t>
+  </si>
+  <si>
+    <t>var userInput3= parseInt(prompt("Please enter the 3rd length of your triangle."));</t>
+  </si>
+  <si>
+    <t>if((userInput1!==userInput2 &amp;&amp; userInput2!==userInput3 &amp;&amp; userInput1!==userInput3) &amp;&amp; (userInput1+userInput2 &gt;userInput3 || userInput1+userInput3 &gt;userInput2 || userInput3+userInput2 &gt;userInput1)&amp;&amp;(userInput1+userInput2 &lt;=userInput3 || userInput1+userInput3 &lt;=userInput2 || userInput3+userInput2 &lt;=userInput1)){alert("Your triangle is a scalene triangle");</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>else{alert("Your triangle is NOT a scalene triangle");}</t>
+  </si>
+  <si>
+    <t>userInput1+userInput2 &gt;userInput3 &amp;&amp; userInput1+userInput3 &gt;userInput2 &amp;&amp; userInput3+userInput2 &gt;userInput1</t>
   </si>
 </sst>
 </file>
@@ -472,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,23 +641,88 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>26</v>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update the js file with algorithm for all conditions
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Behaviour
 The program should:</t>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>userInput1+userInput2 &gt;userInput3 &amp;&amp; userInput1+userInput3 &gt;userInput2 &amp;&amp; userInput3+userInput2 &gt;userInput1</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>(userInput1+userInput2 &gt;userInput3) &amp;&amp; (userInput1+userInput3 &gt;userInput2) &amp;&amp; (userInput3+userInput2 &gt;userInput1</t>
+  </si>
+  <si>
+    <t>check on whether lengths make a triangle</t>
   </si>
 </sst>
 </file>
@@ -500,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,6 +650,11 @@
         <v>29</v>
       </c>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>26</v>
@@ -666,9 +680,24 @@
         <v>40</v>
       </c>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="34" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>